<commit_message>
Basic barplot functionality is in place
</commit_message>
<xml_diff>
--- a/Students/ebuer/termp/datafiles/test_chemistry.xlsx
+++ b/Students/ebuer/termp/datafiles/test_chemistry.xlsx
@@ -10,7 +10,7 @@
     <sheet name="tbl_EXPORT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tbl_EXPORT!$A$1:$AY$3037</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tbl_EXPORT!$A$1:$AY$300</definedName>
     <definedName name="tbl_EXPORT">tbl_EXPORT!$A$1:$AY$3037</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -2131,7 +2131,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>